<commit_message>
Update data and source code files
</commit_message>
<xml_diff>
--- a/data/federalfinancegestion/close_btc_rf_importance.xlsx
+++ b/data/federalfinancegestion/close_btc_rf_importance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -455,12 +455,12 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.7427130037696568</v>
+        <v>0.7427197720461846</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -468,12 +468,12 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.05612242474920228</v>
+        <v>0.05525499609234251</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -481,12 +481,12 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.05509510671706127</v>
+        <v>0.05428660641598676</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -494,12 +494,12 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.05349866907014019</v>
+        <v>0.05331271660789425</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -507,12 +507,12 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.04346416266694544</v>
+        <v>0.03174501312722938</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -520,51 +520,51 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.009591216580155703</v>
+        <v>0.009391783829927705</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Gold</t>
+          <t>doge_tweet_count</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0035369994406562</v>
+        <v>0.007557789928097706</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>EUR003M_Index</t>
+          <t>eth_tweet_count</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.002865391843633994</v>
+        <v>0.005731061429251037</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>US0012M_Index</t>
+          <t>Gold</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.002683209921009334</v>
+        <v>0.003538039414323093</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>49</v>
+        <v>128</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -572,194 +572,194 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.002334373501256381</v>
+        <v>0.002912837004389478</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>VStoxx</t>
+          <t>US0012M_Index</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.001681628295616315</v>
+        <v>0.002526214719919515</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>EUR006M_Index</t>
+          <t>EUR003M_Index</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.001607930010745471</v>
+        <v>0.002209547078184962</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>US0003M_Index</t>
+          <t>VStoxx</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.001578895085244873</v>
+        <v>0.001795599808369886</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Close_XRP</t>
+          <t>EUR006M_Index</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.001529497073075243</v>
+        <v>0.001661243090874504</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TreasuryYield5Years</t>
+          <t>EUR001M_Index</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.001511581701955633</v>
+        <v>0.001648692643225904</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>EUR001M_Index</t>
+          <t>TreasuryYield5Years</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.001470474805994764</v>
+        <v>0.001407063017649868</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>58</v>
+        <v>129</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>H15T5Y_Index</t>
+          <t>US0003M_Index</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.001160438476755391</v>
+        <v>0.001375743707434236</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Brent_CrudeOil</t>
+          <t>Close_XRP</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.001009894137978659</v>
+        <v>0.001243638190166335</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ECRPUS1YIndex</t>
+          <t>H15T5Y_Index</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.001004783404917007</v>
+        <v>0.001240789556097427</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>regulation_attention_twitter</t>
+          <t>Brent_CrudeOil</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.0009523127020612861</v>
+        <v>0.001028162683855781</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>51</v>
+        <v>142</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>US0006M_Index</t>
+          <t>ECRPUS1YIndex</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.0009478824052342973</v>
+        <v>0.0009293358409579281</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Volume_BTC</t>
+          <t>regulation_attention_twitter</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.0006866481778035703</v>
+        <v>0.0007090109170986995</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>InflationBreakevenT5YIE</t>
+          <t>Volume_BTC</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.0005834179887389461</v>
+        <v>0.0006222593838957283</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>uncertainty_attention_twitter</t>
+          <t>US0006M_Index</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.0005819264385034794</v>
+        <v>0.0005485667258514968</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -767,38 +767,38 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.0005589493613531221</v>
+        <v>0.0005333186860946081</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>54</v>
+        <v>154</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>H15T3M_Index</t>
+          <t>VXNCLS</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.0005285955590634268</v>
+        <v>0.0005240514629654836</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>75</v>
+        <v>148</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>VXNCLS</t>
+          <t>13WeeksTreasuryBill</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.0005111526806084934</v>
+        <v>0.0004775013427395016</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -806,298 +806,298 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.0004832466886849924</v>
+        <v>0.0004761019814908038</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>FedSF_NewsSentiment</t>
+          <t>InflationBreakevenT5YIE</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.0004456634009121606</v>
+        <v>0.0004734785356243989</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>PercentHikeCut</t>
+          <t>FedSF_NewsSentiment</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.0004080600061157958</v>
+        <v>0.0003728575081481725</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>cbdc_attention_twitter</t>
+          <t>VIXCLS</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.0003983542976953338</v>
+        <v>0.0003685317989239853</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>btc_tweet_count</t>
+          <t>CDS_ITRXEXE</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.0003941586430630338</v>
+        <v>0.0003516105717096838</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>VIXCLS</t>
+          <t>cbdc_attention_twitter</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.000388860151503475</v>
+        <v>0.0003408262951138827</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>TreasuryYield30Years</t>
+          <t>PercentHikeCut</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.0003859524304276933</v>
+        <v>0.0003356909365427228</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>89</v>
+        <v>151</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CDS_ITRXEXE</t>
+          <t>TreasuryYield30Years</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.0003506003913256913</v>
+        <v>0.0003297223568212274</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>64</v>
+        <v>158</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>WTI_CrudeOil</t>
+          <t>InflationBreakevenT10YIE</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.0003318924117410833</v>
+        <v>0.000327392193605304</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Volume_LTC</t>
+          <t>WTI_CrudeOil</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.0003249270788356097</v>
+        <v>0.0002914450436910687</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>InflationBreakevenT10YIE</t>
+          <t>Volume_LTC</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.0002915741850752766</v>
+        <v>0.00028961868016286</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>regulation_vader_polarity_compound_min</t>
+          <t>H15T1M_Index</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.0002764206944804428</v>
+        <v>0.0002757879493593165</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>CDS_ITRXESE</t>
+          <t>btc_tweet_count</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.000267015072261114</v>
+        <v>0.0002710789225404648</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>H15T10Y_Index</t>
+          <t>crisis_vader_polarity_compound_max</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.0002424299027182688</v>
+        <v>0.0002705381856747025</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>monp_attention_twitter</t>
+          <t>uncertainty_attention_twitter</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.0002423818555393589</v>
+        <v>0.0002393566335780586</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>H15T1M_Index</t>
+          <t>shib_tweet_count</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.0002418626106556652</v>
+        <v>0.000231319674066625</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TwitterMktUncertaintySCA</t>
+          <t>H15T10Y_Index</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.0002279604404461735</v>
+        <v>0.0002136960875606813</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TwitterMktUncertaintyEnglish</t>
+          <t>TwitterMktUncertaintySCA</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.0002251244463472944</v>
+        <v>0.0002131742874162515</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>CDS_ITRXEBE</t>
+          <t>ada_textblob_polarity_min</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.0002159440274050561</v>
+        <v>0.0002003753525474909</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>80</v>
+        <v>169</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>TwitterEcoUncertaintyEnglish</t>
+          <t>CDS_ITRXEBE</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.0002135997428781303</v>
+        <v>0.0001993958151945693</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Volume_BNB</t>
+          <t>ltc_tweet_count</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.0002123483276208745</v>
+        <v>0.0001947392504221976</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>crisis_vader_polarity_compound_max</t>
+          <t>regulation_textblob_polarity_mean</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.0002041969326126136</v>
+        <v>0.0001917646215758015</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>VXVCLS</t>
+          <t>dot_tweet_count</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.0001962325373658297</v>
+        <v>0.0001890871037642019</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>83</v>
+        <v>162</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1105,540 +1105,1567 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.0001786666965746865</v>
+        <v>0.0001879837165756</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>69</v>
+        <v>159</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>13WeeksTreasuryBill</t>
+          <t>TwitterEcoUncertaintyEnglish</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.0001767991518590421</v>
+        <v>0.0001709382672331765</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>monp_textblob_polarity_mean</t>
+          <t>VXVCLS</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.0001618841403441552</v>
+        <v>0.0001623392609884874</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>14</v>
+        <v>167</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Volume_ETH</t>
+          <t>CDS_ITRXEUE</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.000151129678354895</v>
+        <v>0.0001562526660452925</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>USEPUINDXD</t>
+          <t>ada_tweet_count</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.0001175004037526982</v>
+        <v>0.0001350922613323567</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>TwitterMktUncertaintyUSA</t>
+          <t>bch_textblob_polarity_mean</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.000114448205177905</v>
+        <v>0.0001316975736446788</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>regulation_textblob_polarity_mean</t>
+          <t>ltc_textblob_polarity_mean</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.0001132529102000659</v>
+        <v>0.0001310442250519859</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>crisis_textblob_polarity_mean</t>
+          <t>TwitterEcoUncertaintyWGT</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.0001033404802365489</v>
+        <v>0.0001296378786814008</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>88</v>
+        <v>170</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>CDS_ITRXEUE</t>
+          <t>CDS_ITRXESE</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.0001022675767360187</v>
+        <v>0.000125195765590962</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>H15T6M_Index</t>
+          <t>Volume_BNB</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>9.924018040699152e-05</v>
+        <v>0.0001136314803994039</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>sdcc_vader_polarity_compound_min</t>
+          <t>monp_attention_twitter</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>9.885706730762632e-05</v>
+        <v>0.0001132674649674555</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>10</v>
+        <v>133</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>sdcc_attention_twitter</t>
+          <t>H15T3M_Index</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>9.8667105418477e-05</v>
+        <v>0.0001125175911680582</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>59</v>
+        <v>163</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>H15T3Y_Index</t>
+          <t>TwitterMktUncertaintyEnglish</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>9.567688802394444e-05</v>
+        <v>0.000105461137263071</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>56</v>
+        <v>164</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>H15T1Y_Index</t>
+          <t>TwitterMktUncertaintyUSA</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>9.424361046550903e-05</v>
+        <v>0.000105280468205857</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>TwitterEcoUncertaintyUSA</t>
+          <t>Volume_ETH</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>9.011308098529961e-05</v>
+        <v>0.0001032770648787312</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>31</v>
+        <v>134</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>sdcc_vader_polarity_compound_max</t>
+          <t>H15T6M_Index</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>7.963250370223139e-05</v>
+        <v>0.0001000076472587869</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>sdcc_textblob_polarity_mean</t>
+          <t>bnb_textblob_polarity_min</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>7.492239022578184e-05</v>
+        <v>9.879296949531289e-05</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>btc_vader_polarity_compound_max</t>
+          <t>bch_vader_polarity_compound_mean</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>6.261822030014635e-05</v>
+        <v>9.851548170297737e-05</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>sdcc_textblob_polarity_max</t>
+          <t>shib_vader_polarity_compound_max</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>6.185713301133154e-05</v>
+        <v>9.830255040192585e-05</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>TwitterEcoUncertaintyWGT</t>
+          <t>ltc_posts_count</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>6.071057902357984e-05</v>
+        <v>9.256930030557731e-05</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>regulation_textblob_polarity_max</t>
+          <t>monp_textblob_polarity_mean</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>5.926854650603374e-05</v>
+        <v>9.198511680383812e-05</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>crisis_vader_polarity_compound_min</t>
+          <t>btc_vader_polarity_compound_min</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>5.824524862394654e-05</v>
+        <v>8.129231274071963e-05</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>monp_textblob_polarity_min</t>
+          <t>crisis_textblob_polarity_mean</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>5.630053453298525e-05</v>
+        <v>8.01190576924097e-05</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>btc_textblob_polarity_max</t>
+          <t>sdcc_vader_polarity_compound_max</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>5.499233138404558e-05</v>
+        <v>8.000450724218841e-05</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>regulation_vader_polarity_compound_max</t>
+          <t>sdcc_vader_polarity_compound_min</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5.482908647522528e-05</v>
+        <v>7.86312316614691e-05</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>monp_vader_polarity_compound_mean</t>
+          <t>bch_textblob_polarity_min</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>5.439187029039479e-05</v>
+        <v>7.747980310733912e-05</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>sdcc_vader_polarity_compound_mean</t>
+          <t>dot_textblob_polarity_mean</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>5.416731100278002e-05</v>
+        <v>7.626243709299318e-05</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>btc_textblob_polarity_min</t>
+          <t>sol_tweet_count</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>5.41293301386904e-05</v>
+        <v>6.971797022131232e-05</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>H15T2Y_Index</t>
+          <t>btc_textblob_polarity_mean</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>5.408504167534612e-05</v>
+        <v>6.721451206843507e-05</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>btc_vader_polarity_compound_min</t>
+          <t>ada_vader_polarity_compound_min</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>5.244745012276901e-05</v>
+        <v>6.323088678214678e-05</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>crisis_textblob_polarity_min</t>
+          <t>doge_vader_polarity_compound_min</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>5.235872845819556e-05</v>
+        <v>6.056250407680925e-05</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>crisis_vader_polarity_compound_mean</t>
+          <t>doge_textblob_polarity_mean</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4.969302556762355e-05</v>
+        <v>5.897663308716903e-05</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>monp_vader_polarity_compound_max</t>
+          <t>eth_vader_polarity_compound_max</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>4.938368091346182e-05</v>
+        <v>5.892125857439149e-05</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>crisis_textblob_polarity_max</t>
+          <t>TwitterEcoUncertaintyUSA</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>4.869277672035068e-05</v>
+        <v>5.851707587688616e-05</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>TwitterMktUncertaintyWGT</t>
+          <t>monp_vader_polarity_compound_min</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4.642843362473953e-05</v>
+        <v>5.807049223907141e-05</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>monp_vader_polarity_compound_min</t>
+          <t>sdcc_vader_polarity_compound_mean</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>4.610860131355628e-05</v>
+        <v>5.801296432400387e-05</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>monp_textblob_polarity_max</t>
+          <t>ada_vader_polarity_compound_mean</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>4.608462697380945e-05</v>
+        <v>5.767670573047046e-05</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>regulation_vader_polarity_compound_mean</t>
+          <t>bnb_vader_polarity_compound_mean</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>4.595151745737507e-05</v>
+        <v>5.74141493566765e-05</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>6</v>
+        <v>135</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>btc_vader_polarity_compound_mean</t>
+          <t>H15T1Y_Index</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4.22167295833533e-05</v>
+        <v>5.716624777828602e-05</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>btc_textblob_polarity_mean</t>
+          <t>H15T2Y_Index</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>4.203395092958569e-05</v>
+        <v>5.334935846944601e-05</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>regulation_textblob_polarity_min</t>
+          <t>sol_vader_polarity_compound_max</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>3.46565499966179e-05</v>
+        <v>5.27226220336384e-05</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>27</v>
+        <v>123</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
+          <t>regulation_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>5.257785603662359e-05</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>sol_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>5.168398759691802e-05</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>sol_textblob_polarity_mean</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>5.16746250636371e-05</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>bnb_tweet_count</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>5.156771552426541e-05</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>ltc_vader_polarity_compound_min</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>4.972144971977155e-05</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>regulation_posts_count</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>4.937052812970078e-05</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>ltc_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>4.848097188202467e-05</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>TwitterMktUncertaintyWGT</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>4.740194634354276e-05</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>ltc_vader_polarity_compound_max</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>4.455670166597426e-05</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>crisis_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>4.411349825106804e-05</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>monp_posts_count</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>4.385801407723568e-05</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>bnb_vader_polarity_compound_max</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>4.349414788597694e-05</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>monp_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>4.245382518622586e-05</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>H15T3Y_Index</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>4.213015862357062e-05</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>sdcc_attention_twitter</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>4.210270718567645e-05</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>shib_textblob_polarity_mean</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>4.173695057085054e-05</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>USEPUINDXD</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>4.170754098058757e-05</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>ltc_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>4.139938457068283e-05</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>bch_vader_polarity_compound_max</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>4.066345994749089e-05</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>eth_textblob_polarity_mean</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>3.987572535177814e-05</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>crisis_posts_count</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>3.929128669540713e-05</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>shib_vader_polarity_compound_min</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>3.908452830727907e-05</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>regulation_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>3.865461304568672e-05</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>sdcc_textblob_polarity_mean</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>3.799198356046157e-05</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>dot_vader_polarity_compound_max</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>3.793869056820382e-05</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>shib_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>3.764209112532719e-05</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>bnb_textblob_polarity_mean</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>3.706741134306212e-05</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>sdcc_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>3.610605761173171e-05</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
           <t>sdcc_textblob_polarity_min</t>
         </is>
       </c>
-      <c r="C93" t="n">
-        <v>2.833378452377342e-05</v>
+      <c r="C121" t="n">
+        <v>3.585908195706809e-05</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>shib_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>3.515453890021382e-05</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>regulation_vader_polarity_compound_max</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>3.473124635648048e-05</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>bch_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>3.354483753962432e-05</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>crisis_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>3.344698543021866e-05</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>regulation_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>3.30685542659779e-05</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>doge_vader_polarity_compound_max</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>3.304956915242724e-05</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>bnb_vader_polarity_compound_min</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>3.293595370942277e-05</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>eth_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>3.267810625137209e-05</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>dot_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>3.251048921532603e-05</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>shib_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>3.235517512791573e-05</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>doge_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>3.130889129819427e-05</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>dot_posts_count</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>3.056906190302947e-05</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>btc_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>3.048005779485274e-05</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>dot_vader_polarity_compound_min</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>3.036443305237146e-05</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>xrp_tweet_count</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>3.030083501751935e-05</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>btc_vader_polarity_compound_max</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>2.960777598735615e-05</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>ada_posts_count</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>2.934643768403104e-05</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>sol_vader_polarity_compound_min</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>2.931723368263232e-05</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>ada_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>2.891690852866586e-05</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>matic_tweet_count</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>2.854400908479426e-05</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>crisis_vader_polarity_compound_min</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>2.852105985394224e-05</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>eth_vader_polarity_compound_min</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>2.843137096757068e-05</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>btc_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>2.812994709182676e-05</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>monp_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>2.770677958879053e-05</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>dot_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>2.696413701464022e-05</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>regulation_vader_polarity_compound_min</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>2.606357978212704e-05</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>doge_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>2.569005491943139e-05</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>ltc_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>2.518304015152483e-05</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>monp_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>2.421437311244127e-05</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>bch_tweet_count</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>2.325577574360991e-05</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>bch_vader_polarity_compound_min</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>2.29908976734373e-05</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>sol_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>2.298444973880834e-05</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>doge_posts_count</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>2.280615278411185e-05</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>btc_posts_count</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>2.225547927363583e-05</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>eth_posts_count</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>2.213421074476491e-05</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>doge_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>2.195562549385994e-05</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>ada_textblob_polarity_mean</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>2.177475046270658e-05</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>btc_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>2.148038513990168e-05</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>eth_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>2.114308293572673e-05</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>crisis_vader_polarity_compound_mean</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>2.112162963858341e-05</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>bnb_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>2.10907020990819e-05</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>ada_vader_polarity_compound_max</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>2.103152747572185e-05</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>monp_vader_polarity_compound_max</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>1.985445202327906e-05</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>sol_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>1.901205881108513e-05</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>eth_textblob_polarity_max</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>1.857948957062319e-05</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>bnb_posts_count</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>1.823377247289304e-05</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>bch_posts_count</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>1.82043761228067e-05</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>dot_textblob_polarity_min</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>1.492103782858722e-05</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>sdcc_posts_count</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>1.218910150591379e-05</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>shib_posts_count</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>1.080783566788255e-05</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>sol_posts_count</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>1.075367082684318e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>